<commit_message>
added socket downloading for schematic at startup
downloads the latest schematic on startup from the :
localhost:80/test.html
</commit_message>
<xml_diff>
--- a/Documentation/Implmented Nodes.xlsx
+++ b/Documentation/Implmented Nodes.xlsx
@@ -1,17 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="480" yWindow="810" windowWidth="14775" windowHeight="7080"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Tabellenblatt1" sheetId="1" r:id="rId3"/>
+    <sheet name="Tabellenblatt1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="155">
   <si>
     <t>Class Name</t>
   </si>
@@ -323,29 +326,189 @@
   </si>
   <si>
     <t>OpenWeatherMap</t>
+  </si>
+  <si>
+    <t>node_simplemath</t>
+  </si>
+  <si>
+    <t>Base Calc</t>
+  </si>
+  <si>
+    <t>[0,float, value 1][1,float, value 2]</t>
+  </si>
+  <si>
+    <t>[2,float,output value]</t>
+  </si>
+  <si>
+    <t>&lt;math_operation (add,sub,mul,dif,mod,min,max,pow,dim)&gt;%</t>
+  </si>
+  <si>
+    <t>XML NSI</t>
+  </si>
+  <si>
+    <t>nbdi</t>
+  </si>
+  <si>
+    <t>nbdo</t>
+  </si>
+  <si>
+    <t>bndmx</t>
+  </si>
+  <si>
+    <t>bnidisp</t>
+  </si>
+  <si>
+    <t>bland</t>
+  </si>
+  <si>
+    <t>blor</t>
+  </si>
+  <si>
+    <t>blxor</t>
+  </si>
+  <si>
+    <t>blnot</t>
+  </si>
+  <si>
+    <t>blbuffer</t>
+  </si>
+  <si>
+    <t>bifte</t>
+  </si>
+  <si>
+    <t>biftest</t>
+  </si>
+  <si>
+    <t>biftefl</t>
+  </si>
+  <si>
+    <t>intcomp</t>
+  </si>
+  <si>
+    <t>floatcomp</t>
+  </si>
+  <si>
+    <t>strcomp</t>
+  </si>
+  <si>
+    <t>blfrs</t>
+  </si>
+  <si>
+    <t>blft</t>
+  </si>
+  <si>
+    <t>nbcoin</t>
+  </si>
+  <si>
+    <t>nbcost</t>
+  </si>
+  <si>
+    <t>nbcofl</t>
+  </si>
+  <si>
+    <t>nbcobot</t>
+  </si>
+  <si>
+    <t>nbsttoi</t>
+  </si>
+  <si>
+    <t>nbsttof</t>
+  </si>
+  <si>
+    <t>nbitof</t>
+  </si>
+  <si>
+    <t>nbftoi</t>
+  </si>
+  <si>
+    <t>nbinttostr</t>
+  </si>
+  <si>
+    <t>nbfltostr</t>
+  </si>
+  <si>
+    <t>ctimest</t>
+  </si>
+  <si>
+    <t>tstoint</t>
+  </si>
+  <si>
+    <t>basetimer</t>
+  </si>
+  <si>
+    <t>phhlux</t>
+  </si>
+  <si>
+    <t>opwemare</t>
+  </si>
+  <si>
+    <t>simplemath</t>
+  </si>
+  <si>
+    <t>node_basiccounter</t>
+  </si>
+  <si>
+    <t>basiccounter</t>
+  </si>
+  <si>
+    <t>Basic Counter</t>
+  </si>
+  <si>
+    <t>[0,bool, trigger][1,float, inc_value][2,bool, set_zero]</t>
+  </si>
+  <si>
+    <t>[3,float,output value]</t>
+  </si>
+  <si>
+    <t>Performs basic math operations</t>
+  </si>
+  <si>
+    <t>[0,value,channel_value]</t>
+  </si>
+  <si>
+    <t>[0,string,line_string]</t>
+  </si>
+  <si>
+    <t>&lt;mid&gt;%&lt;msi&gt;%&lt;line_number&gt;%</t>
+  </si>
+  <si>
+    <t>&lt;mid&gt;%&lt;msi&gt;%&lt;channel&gt;%</t>
+  </si>
+  <si>
+    <t>Writes a string to the selected row of the Display Extenttion if you choose as mid 0 you can write to the intern dispaly</t>
+  </si>
+  <si>
+    <t>Write a Value to the dmx bux please use as mid: 0 to use ther internal dmx interface</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="5">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
+      <name val="Arial"/>
     </font>
-    <font/>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF222222"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="5">
@@ -353,7 +516,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -380,6 +543,7 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left/>
@@ -388,94 +552,371 @@
         <color rgb="FFAAAAAA"/>
       </top>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+  <cellXfs count="11">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AB44"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="22.29"/>
-    <col customWidth="1" min="5" max="5" width="39.0"/>
-    <col customWidth="1" min="6" max="6" width="24.86"/>
-    <col customWidth="1" min="7" max="7" width="61.86"/>
-    <col customWidth="1" min="8" max="8" width="33.57"/>
-    <col customWidth="1" min="9" max="9" width="40.14"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="6" max="6" width="39" customWidth="1"/>
+    <col min="7" max="7" width="24.85546875" customWidth="1"/>
+    <col min="8" max="8" width="61.85546875" customWidth="1"/>
+    <col min="9" max="9" width="33.5703125" customWidth="1"/>
+    <col min="10" max="10" width="52.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:28">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>109</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
@@ -492,767 +933,950 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
       <c r="AA1" s="2"/>
-    </row>
-    <row r="2">
+      <c r="AB1" s="2"/>
+    </row>
+    <row r="2" spans="1:28" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="3" t="b">
-        <v>1</v>
-      </c>
       <c r="D2" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:28" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="3" t="b">
-        <v>1</v>
-      </c>
       <c r="D3" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:28" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="3" t="b">
-        <v>1</v>
-      </c>
       <c r="D4" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5">
+      <c r="H4" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" ht="15.75" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="3" t="b">
-        <v>1</v>
-      </c>
       <c r="D5" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6">
+      <c r="H5" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" ht="15.75" customHeight="1">
       <c r="A6" s="3"/>
-    </row>
-    <row r="7">
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:28" ht="15.75" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="3" t="b">
-        <v>0</v>
-      </c>
       <c r="D7" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E7" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>28</v>
+      <c r="F7" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="G7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="I7" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:28" ht="15.75" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="3" t="b">
-        <v>0</v>
-      </c>
       <c r="D8" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E8" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>28</v>
+      <c r="F8" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="G8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="I8" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:28" ht="15.75" customHeight="1">
       <c r="A9" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="3" t="b">
-        <v>0</v>
-      </c>
       <c r="D9" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E9" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>28</v>
+      <c r="F9" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="G9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="I9" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="I9" s="5"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="7"/>
-    </row>
-    <row r="10">
+      <c r="J9" s="5"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="7"/>
+    </row>
+    <row r="10" spans="1:28" ht="15.75" customHeight="1">
       <c r="A10" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="3" t="b">
-        <v>0</v>
-      </c>
       <c r="D10" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="E10" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>28</v>
+      <c r="E10" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="G10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="I10" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:28" ht="15.75" customHeight="1">
       <c r="A11" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="3" t="b">
-        <v>0</v>
-      </c>
       <c r="D11" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E11" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>28</v>
+      <c r="F11" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="G11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="I11" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:28" ht="15.75" customHeight="1">
       <c r="A13" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="3" t="b">
-        <v>0</v>
-      </c>
       <c r="D13" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E13" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G13" s="4" t="s">
+      <c r="F13" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="I13" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:28" ht="15.75" customHeight="1">
       <c r="A14" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="3" t="b">
-        <v>0</v>
-      </c>
       <c r="D14" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E14" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G14" s="4" t="s">
+      <c r="F14" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="I14" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:28" ht="15.75" customHeight="1">
       <c r="A15" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="3" t="b">
-        <v>0</v>
-      </c>
       <c r="D15" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E15" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G15" s="4" t="s">
+      <c r="F15" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H15" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="I15" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="A17" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="3" t="b">
-        <v>0</v>
-      </c>
       <c r="D17" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E17" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18">
+      <c r="F17" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" s="3" t="s">
         <v>55</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="3" t="b">
-        <v>0</v>
-      </c>
       <c r="D18" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E18" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19">
+      <c r="F18" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="A19" s="3" t="s">
         <v>57</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C19" s="3" t="b">
-        <v>0</v>
-      </c>
       <c r="D19" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E19" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21">
+      <c r="F19" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="A21" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="3" t="b">
-        <v>0</v>
-      </c>
       <c r="D21" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E21" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="F21" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22">
+      <c r="F21" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="A22" s="3" t="s">
         <v>61</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C22" s="3" t="b">
-        <v>0</v>
-      </c>
       <c r="D22" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E22" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="F22" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24">
+      <c r="F22" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" customHeight="1">
       <c r="A24" s="3" t="s">
         <v>63</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="3" t="b">
-        <v>0</v>
-      </c>
       <c r="D24" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25">
+        <v>1</v>
+      </c>
+      <c r="F24" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" customHeight="1">
       <c r="A25" s="3" t="s">
         <v>65</v>
       </c>
       <c r="B25" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C25" s="3" t="b">
-        <v>0</v>
-      </c>
       <c r="D25" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26">
+        <v>1</v>
+      </c>
+      <c r="F25" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" customHeight="1">
       <c r="A26" s="3" t="s">
         <v>67</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C26" s="3" t="b">
-        <v>0</v>
-      </c>
       <c r="D26" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27">
+        <v>1</v>
+      </c>
+      <c r="F26" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" customHeight="1">
       <c r="A27" s="3" t="s">
         <v>69</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C27" s="3" t="b">
-        <v>0</v>
-      </c>
       <c r="D27" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E27" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28">
+        <v>1</v>
+      </c>
+      <c r="F27" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" customHeight="1">
       <c r="A28" s="3" t="s">
         <v>71</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C28" s="3" t="b">
-        <v>0</v>
-      </c>
       <c r="D28" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30">
+        <v>1</v>
+      </c>
+      <c r="F28" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" customHeight="1">
       <c r="A30" s="3" t="s">
         <v>73</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C30" s="3" t="b">
-        <v>0</v>
-      </c>
       <c r="D30" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E30" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31">
+        <v>0</v>
+      </c>
+      <c r="F30" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" customHeight="1">
       <c r="A31" s="3" t="s">
         <v>75</v>
       </c>
       <c r="B31" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C31" s="3" t="b">
-        <v>0</v>
-      </c>
       <c r="D31" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E31" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="32">
+        <v>0</v>
+      </c>
+      <c r="F31" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" customHeight="1">
       <c r="A32" s="3" t="s">
         <v>77</v>
       </c>
       <c r="B32" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C32" s="3" t="b">
-        <v>0</v>
-      </c>
       <c r="D32" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E32" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="33">
+        <v>0</v>
+      </c>
+      <c r="F32" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="15.75" customHeight="1">
       <c r="A33" s="3" t="s">
         <v>79</v>
       </c>
       <c r="B33" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C33" s="3" t="b">
-        <v>0</v>
-      </c>
       <c r="D33" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E33" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="34">
+        <v>0</v>
+      </c>
+      <c r="F33" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="15.75" customHeight="1">
       <c r="A34" s="3" t="s">
         <v>81</v>
       </c>
       <c r="B34" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C34" s="3" t="b">
-        <v>0</v>
-      </c>
       <c r="D34" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E34" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="35">
+        <v>0</v>
+      </c>
+      <c r="F34" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="15.75" customHeight="1">
       <c r="A35" s="3" t="s">
         <v>82</v>
       </c>
       <c r="B35" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C35" s="3" t="b">
-        <v>0</v>
-      </c>
       <c r="D35" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E35" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="37">
+        <v>0</v>
+      </c>
+      <c r="F35" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="15.75" customHeight="1">
       <c r="A37" s="3" t="s">
         <v>84</v>
       </c>
       <c r="B37" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C37" s="3" t="b">
-        <v>0</v>
-      </c>
       <c r="D37" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E37" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="F37" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H37" s="4" t="s">
+      <c r="F37" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I37" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="J37" s="3" t="s">
+      <c r="K37" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:11" ht="15.75" customHeight="1">
       <c r="A38" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B38" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C38" s="3" t="b">
-        <v>0</v>
-      </c>
       <c r="D38" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E38" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J38" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F38" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K38" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:11" ht="15.75" customHeight="1">
       <c r="A39" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B39" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C39" s="3" t="b">
-        <v>0</v>
-      </c>
       <c r="D39" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E39" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="F39" s="3" t="s">
-        <v>28</v>
+      <c r="F39" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="G39" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H39" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="H39" s="3" t="s">
+      <c r="I39" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="J39" s="3" t="s">
+      <c r="K39" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:11" ht="15.75" customHeight="1">
       <c r="A40" s="3" t="s">
         <v>96</v>
       </c>
       <c r="B40" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C40" s="3" t="b">
-        <v>0</v>
-      </c>
       <c r="D40" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E40" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="F40" s="3" t="s">
+      <c r="F40" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G40" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="G40" s="4" t="s">
+      <c r="H40" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="I40" s="3" t="s">
+      <c r="J40" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="J40" s="3" t="s">
+      <c r="K40" s="3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:11" ht="15.75" customHeight="1">
       <c r="A41" s="3" t="s">
         <v>102</v>
       </c>
       <c r="B41" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C41" s="3" t="b">
-        <v>0</v>
-      </c>
       <c r="D41" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E41" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>28</v>
+        <v>0</v>
+      </c>
+      <c r="F41" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A43" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D43" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E43" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F43" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H43" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="I43" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="J43" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="K43" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A44" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D44" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E44" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F44" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H44" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="I44" s="9" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added som colors to excel list
</commit_message>
<xml_diff>
--- a/Documentation/Implmented Nodes.xlsx
+++ b/Documentation/Implmented Nodes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="209">
   <si>
     <t>Class Name</t>
   </si>
@@ -632,13 +632,22 @@
   </si>
   <si>
     <t>&lt;operation (==, !=)&gt;%</t>
+  </si>
+  <si>
+    <t>All setters implemented</t>
+  </si>
+  <si>
+    <t>A standard AND-Gate. If both inputs are true. The output is true too</t>
+  </si>
+  <si>
+    <t>A standard OR-Gate. If only one of the inputs  true. The output is true too</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -663,8 +672,14 @@
       <color rgb="FF222222"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="2" tint="-9.9978637043366805E-2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -689,8 +704,20 @@
         <bgColor rgb="FF6D9EEB"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -698,40 +725,64 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1028,10 +1079,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC39"/>
+  <dimension ref="A1:AD39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1041,15 +1092,16 @@
     <col min="3" max="3" width="23.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.28515625" style="2" customWidth="1"/>
     <col min="5" max="6" width="14.42578125" style="2"/>
-    <col min="7" max="7" width="39" style="2" customWidth="1"/>
-    <col min="8" max="8" width="24.85546875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="61.85546875" style="2" customWidth="1"/>
-    <col min="10" max="10" width="68" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="52.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="14.42578125" style="2"/>
+    <col min="7" max="7" width="27.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="39" style="2" customWidth="1"/>
+    <col min="9" max="9" width="24.85546875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="61.85546875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="68" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="52.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="14.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:30">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1069,24 +1121,26 @@
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
@@ -1103,8 +1157,9 @@
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
-    </row>
-    <row r="2" spans="1:29" ht="15.75" customHeight="1">
+      <c r="AD1" s="1"/>
+    </row>
+    <row r="2" spans="1:30" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -1124,22 +1179,26 @@
         <v>0</v>
       </c>
       <c r="G2" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="11"/>
+      <c r="K2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="15.75" customHeight="1">
+    <row r="3" spans="1:30" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
@@ -1159,22 +1218,26 @@
         <v>0</v>
       </c>
       <c r="G3" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="10"/>
+      <c r="L3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="15.75" customHeight="1">
+    <row r="4" spans="1:30" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>21</v>
       </c>
@@ -1194,22 +1257,26 @@
         <v>0</v>
       </c>
       <c r="G4" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="J4" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="11"/>
+      <c r="L4" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="M4" s="4" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="15.75" customHeight="1">
+    <row r="5" spans="1:30" ht="15.75" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>24</v>
       </c>
@@ -1229,22 +1296,26 @@
         <v>0</v>
       </c>
       <c r="G5" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="J5" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="K5" s="11"/>
+      <c r="L5" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="M5" s="4" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="15.75" customHeight="1">
+    <row r="6" spans="1:30" ht="15.75" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>26</v>
       </c>
@@ -1264,19 +1335,26 @@
         <v>0</v>
       </c>
       <c r="G6" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>28</v>
+        <v>1</v>
+      </c>
+      <c r="H6" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="I6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="K6" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:29" ht="15.75" customHeight="1">
+      <c r="L6" s="11"/>
+      <c r="M6" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" ht="15.75" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>31</v>
       </c>
@@ -1296,19 +1374,26 @@
         <v>0</v>
       </c>
       <c r="G7" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>28</v>
+        <v>1</v>
+      </c>
+      <c r="H7" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="I7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="K7" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:29" ht="15.75" customHeight="1">
+      <c r="L7" s="11"/>
+      <c r="M7" s="4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" ht="15.75" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>33</v>
       </c>
@@ -1328,22 +1413,25 @@
         <v>0</v>
       </c>
       <c r="G8" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>28</v>
+        <v>1</v>
+      </c>
+      <c r="H8" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="I8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="K8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="K8" s="6"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="8"/>
-    </row>
-    <row r="9" spans="1:29" ht="15.75" customHeight="1">
+      <c r="L8" s="12"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="7"/>
+    </row>
+    <row r="9" spans="1:30" ht="15.75" customHeight="1">
       <c r="A9" s="3" t="s">
         <v>35</v>
       </c>
@@ -1362,20 +1450,24 @@
       <c r="F9" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="G9" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>28</v>
+      <c r="G9" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="I9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J9" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="J9" s="9" t="s">
+      <c r="K9" s="9" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="10" spans="1:29" ht="15.75" customHeight="1">
+      <c r="L9" s="11"/>
+    </row>
+    <row r="10" spans="1:30" ht="15.75" customHeight="1">
       <c r="A10" s="3" t="s">
         <v>39</v>
       </c>
@@ -1395,19 +1487,23 @@
         <v>0</v>
       </c>
       <c r="G10" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>28</v>
+        <v>1</v>
+      </c>
+      <c r="H10" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="I10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J10" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="K10" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="11" spans="1:29" ht="15.75" customHeight="1">
+      <c r="L10" s="11"/>
+    </row>
+    <row r="11" spans="1:30" ht="15.75" customHeight="1">
       <c r="A11" s="3" t="s">
         <v>41</v>
       </c>
@@ -1427,20 +1523,23 @@
         <v>0</v>
       </c>
       <c r="G11" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H11" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J11" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="K11" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="K11" s="4"/>
-    </row>
-    <row r="12" spans="1:29" ht="15.75" customHeight="1">
+      <c r="L11" s="13"/>
+    </row>
+    <row r="12" spans="1:30" ht="15.75" customHeight="1">
       <c r="A12" s="3" t="s">
         <v>45</v>
       </c>
@@ -1460,19 +1559,23 @@
         <v>0</v>
       </c>
       <c r="G12" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H12" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J12" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="J12" s="5" t="s">
+      <c r="K12" s="5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="13" spans="1:29" ht="15.75" customHeight="1">
+      <c r="L12" s="11"/>
+    </row>
+    <row r="13" spans="1:30" ht="15.75" customHeight="1">
       <c r="A13" s="3" t="s">
         <v>49</v>
       </c>
@@ -1492,19 +1595,23 @@
         <v>0</v>
       </c>
       <c r="G13" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H13" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J13" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="J13" s="5" t="s">
+      <c r="K13" s="5" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="14" spans="1:29" ht="15.75" customHeight="1">
+      <c r="L13" s="11"/>
+    </row>
+    <row r="14" spans="1:30" ht="15.75" customHeight="1">
       <c r="A14" s="3" t="s">
         <v>53</v>
       </c>
@@ -1524,22 +1631,25 @@
         <v>0</v>
       </c>
       <c r="G14" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I14" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H14" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J14" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="K14" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="L14" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="15" spans="1:29" ht="15.75" customHeight="1">
+    <row r="15" spans="1:30" ht="15.75" customHeight="1">
       <c r="A15" s="3" t="s">
         <v>55</v>
       </c>
@@ -1559,22 +1669,25 @@
         <v>0</v>
       </c>
       <c r="G15" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H15" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J15" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="J15" s="4" t="s">
+      <c r="K15" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="L15" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="16" spans="1:29" ht="15.75" customHeight="1">
+    <row r="16" spans="1:30" ht="15.75" customHeight="1">
       <c r="A16" s="3" t="s">
         <v>57</v>
       </c>
@@ -1594,22 +1707,25 @@
         <v>0</v>
       </c>
       <c r="G16" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I16" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H16" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J16" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="J16" s="4" t="s">
+      <c r="K16" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="K16" s="4" t="s">
+      <c r="L16" s="4" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="15.75" customHeight="1">
+    <row r="17" spans="1:13" ht="15.75" customHeight="1">
       <c r="A17" s="3" t="s">
         <v>59</v>
       </c>
@@ -1629,19 +1745,23 @@
         <v>0</v>
       </c>
       <c r="G17" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I17" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H17" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J17" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="J17" s="4" t="s">
+      <c r="K17" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" ht="15.75" customHeight="1">
+      <c r="L17" s="11"/>
+    </row>
+    <row r="18" spans="1:13" ht="15.75" customHeight="1">
       <c r="A18" s="3" t="s">
         <v>61</v>
       </c>
@@ -1661,19 +1781,23 @@
         <v>0</v>
       </c>
       <c r="G18" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I18" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H18" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J18" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="J18" s="4" t="s">
+      <c r="K18" s="4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" ht="15.75" customHeight="1">
+      <c r="L18" s="11"/>
+    </row>
+    <row r="19" spans="1:13" ht="15.75" customHeight="1">
       <c r="A19" s="3" t="s">
         <v>63</v>
       </c>
@@ -1693,19 +1817,23 @@
         <v>1</v>
       </c>
       <c r="G19" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J19" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H19" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J19" s="11"/>
+      <c r="K19" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="K19" s="4" t="s">
+      <c r="L19" s="4" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="15.75" customHeight="1">
+    <row r="20" spans="1:13" ht="15.75" customHeight="1">
       <c r="A20" s="3" t="s">
         <v>65</v>
       </c>
@@ -1725,19 +1853,23 @@
         <v>1</v>
       </c>
       <c r="G20" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H20" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J20" s="11"/>
+      <c r="K20" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="K20" s="4" t="s">
+      <c r="L20" s="4" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15.75" customHeight="1">
+    <row r="21" spans="1:13" ht="15.75" customHeight="1">
       <c r="A21" s="3" t="s">
         <v>67</v>
       </c>
@@ -1757,19 +1889,23 @@
         <v>1</v>
       </c>
       <c r="G21" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J21" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H21" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J21" s="11"/>
+      <c r="K21" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="K21" s="4" t="s">
+      <c r="L21" s="4" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="15.75" customHeight="1">
+    <row r="22" spans="1:13" ht="15.75" customHeight="1">
       <c r="A22" s="3" t="s">
         <v>69</v>
       </c>
@@ -1789,16 +1925,21 @@
         <v>1</v>
       </c>
       <c r="G22" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J22" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H22" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J22" s="11"/>
+      <c r="K22" s="4" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" ht="15.75" customHeight="1">
+      <c r="L22" s="11"/>
+    </row>
+    <row r="23" spans="1:13" ht="15.75" customHeight="1">
       <c r="A23" s="3" t="s">
         <v>71</v>
       </c>
@@ -1818,16 +1959,21 @@
         <v>1</v>
       </c>
       <c r="G23" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J23" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H23" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J23" s="11"/>
+      <c r="K23" s="4" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" ht="15.75" customHeight="1">
+      <c r="L23" s="11"/>
+    </row>
+    <row r="24" spans="1:13" ht="15.75" customHeight="1">
       <c r="A24" s="3" t="s">
         <v>73</v>
       </c>
@@ -1849,17 +1995,21 @@
       <c r="G24" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H24" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I24" s="4" t="s">
+      <c r="H24" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J24" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="J24" s="4" t="s">
+      <c r="K24" s="4" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" ht="15.75" customHeight="1">
+      <c r="L24" s="11"/>
+    </row>
+    <row r="25" spans="1:13" ht="15.75" customHeight="1">
       <c r="A25" s="3" t="s">
         <v>75</v>
       </c>
@@ -1881,17 +2031,21 @@
       <c r="G25" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H25" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I25" s="4" t="s">
+      <c r="H25" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J25" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="J25" s="4" t="s">
+      <c r="K25" s="4" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" ht="15.75" customHeight="1">
+      <c r="L25" s="11"/>
+    </row>
+    <row r="26" spans="1:13" ht="15.75" customHeight="1">
       <c r="A26" s="3" t="s">
         <v>77</v>
       </c>
@@ -1913,17 +2067,21 @@
       <c r="G26" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H26" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I26" s="4" t="s">
+      <c r="H26" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J26" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="J26" s="2" t="s">
+      <c r="K26" s="2" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" ht="15.75" customHeight="1">
+      <c r="L26" s="11"/>
+    </row>
+    <row r="27" spans="1:13" ht="15.75" customHeight="1">
       <c r="A27" s="3" t="s">
         <v>79</v>
       </c>
@@ -1945,17 +2103,21 @@
       <c r="G27" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H27" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I27" s="4" t="s">
+      <c r="H27" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J27" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="J27" s="4" t="s">
+      <c r="K27" s="4" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" ht="15.75" customHeight="1">
+      <c r="L27" s="11"/>
+    </row>
+    <row r="28" spans="1:13" ht="15.75" customHeight="1">
       <c r="A28" s="3" t="s">
         <v>81</v>
       </c>
@@ -1977,17 +2139,21 @@
       <c r="G28" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H28" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I28" s="4" t="s">
+      <c r="H28" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J28" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="J28" s="2" t="s">
+      <c r="K28" s="2" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" ht="15.75" customHeight="1">
+      <c r="L28" s="11"/>
+    </row>
+    <row r="29" spans="1:13" ht="15.75" customHeight="1">
       <c r="A29" s="3" t="s">
         <v>82</v>
       </c>
@@ -2009,17 +2175,21 @@
       <c r="G29" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H29" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I29" s="4" t="s">
+      <c r="H29" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J29" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="J29" s="2" t="s">
+      <c r="K29" s="2" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" ht="15.75" customHeight="1">
+      <c r="L29" s="11"/>
+    </row>
+    <row r="30" spans="1:13" ht="15.75" customHeight="1">
       <c r="A30" s="3" t="s">
         <v>84</v>
       </c>
@@ -2039,19 +2209,24 @@
         <v>0</v>
       </c>
       <c r="G30" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J30" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H30" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J30" s="11"/>
+      <c r="K30" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="L30" s="3" t="s">
+      <c r="L30" s="11"/>
+      <c r="M30" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="15.75" customHeight="1">
+    <row r="31" spans="1:13" ht="15.75" customHeight="1">
       <c r="A31" s="3" t="s">
         <v>88</v>
       </c>
@@ -2073,20 +2248,23 @@
       <c r="G31" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H31" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I31" s="4" t="s">
+      <c r="H31" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J31" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="J31" s="4" t="s">
+      <c r="K31" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="L31" s="3" t="s">
+      <c r="M31" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="15.75" customHeight="1">
+    <row r="32" spans="1:13" ht="15.75" customHeight="1">
       <c r="A32" s="3" t="s">
         <v>91</v>
       </c>
@@ -2106,22 +2284,26 @@
         <v>0</v>
       </c>
       <c r="G32" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>28</v>
+        <v>1</v>
+      </c>
+      <c r="H32" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="I32" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J32" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="J32" s="3" t="s">
+      <c r="K32" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="L32" s="3" t="s">
+      <c r="L32" s="11"/>
+      <c r="M32" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="15.75" customHeight="1">
+    <row r="33" spans="1:13" ht="15.75" customHeight="1">
       <c r="A33" s="3" t="s">
         <v>96</v>
       </c>
@@ -2141,22 +2323,26 @@
         <v>0</v>
       </c>
       <c r="G33" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H33" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H33" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I33" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="I33" s="9" t="s">
+      <c r="J33" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="K33" s="3" t="s">
+      <c r="K33" s="11"/>
+      <c r="L33" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="L33" s="3" t="s">
+      <c r="M33" s="3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="15.75" customHeight="1">
+    <row r="34" spans="1:13" ht="15.75" customHeight="1">
       <c r="A34" s="3" t="s">
         <v>102</v>
       </c>
@@ -2178,20 +2364,23 @@
       <c r="G34" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H34" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I34" s="4" t="s">
+      <c r="H34" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J34" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="J34" s="4" t="s">
+      <c r="K34" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="K34" s="4" t="s">
+      <c r="L34" s="4" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="15.75" customHeight="1">
+    <row r="35" spans="1:13" ht="15.75" customHeight="1">
       <c r="A35" s="3" t="s">
         <v>104</v>
       </c>
@@ -2213,23 +2402,26 @@
       <c r="G35" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H35" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I35" s="4" t="s">
+      <c r="H35" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J35" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="J35" s="9" t="s">
+      <c r="K35" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="K35" s="3" t="s">
+      <c r="L35" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="L35" s="3" t="s">
+      <c r="M35" s="3" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="15.75" customHeight="1">
+    <row r="36" spans="1:13" ht="15.75" customHeight="1">
       <c r="A36" s="3" t="s">
         <v>143</v>
       </c>
@@ -2251,17 +2443,21 @@
       <c r="G36" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H36" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I36" s="4" t="s">
+      <c r="H36" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J36" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="J36" s="4" t="s">
+      <c r="K36" s="4" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" ht="15.75" customHeight="1">
+      <c r="L36" s="11"/>
+    </row>
+    <row r="37" spans="1:13" ht="15.75" customHeight="1">
       <c r="A37" s="3" t="s">
         <v>156</v>
       </c>
@@ -2281,22 +2477,26 @@
         <v>0</v>
       </c>
       <c r="G37" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H37" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I37" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H37" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J37" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="J37" s="4" t="s">
+      <c r="K37" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="L37" s="4" t="s">
+      <c r="L37" s="11"/>
+      <c r="M37" s="4" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="15.75" customHeight="1">
+    <row r="38" spans="1:13" ht="15.75" customHeight="1">
       <c r="A38" s="4" t="s">
         <v>184</v>
       </c>
@@ -2315,20 +2515,24 @@
       <c r="F38" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="G38" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H38" s="4" t="s">
-        <v>28</v>
+      <c r="G38" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H38" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="I38" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J38" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="J38" s="4" t="s">
+      <c r="K38" s="4" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" ht="15.75" customHeight="1">
+      <c r="L38" s="11"/>
+    </row>
+    <row r="39" spans="1:13" ht="15.75" customHeight="1">
       <c r="A39" s="4" t="s">
         <v>185</v>
       </c>
@@ -2347,23 +2551,27 @@
       <c r="F39" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="G39" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H39" s="4" t="s">
-        <v>28</v>
+      <c r="G39" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H39" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="I39" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J39" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="J39" s="4" t="s">
+      <c r="K39" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="K39" s="4" t="s">
+      <c r="L39" s="4" t="s">
         <v>186</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
remove bug in xls
</commit_message>
<xml_diff>
--- a/Documentation/Implmented Nodes.xlsx
+++ b/Documentation/Implmented Nodes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="223">
   <si>
     <t>Class Name</t>
   </si>
@@ -319,9 +319,6 @@
     <t>&lt;bridge-ip&gt;%&lt;username(md5)%lamp_if(1-50)%</t>
   </si>
   <si>
-    <t>Control your Philips Hue Lux Lamps (white only)</t>
-  </si>
-  <si>
     <t>node_opwemare</t>
   </si>
   <si>
@@ -460,9 +457,6 @@
     <t>[3,float,output value]</t>
   </si>
   <si>
-    <t>Performs basic math operations</t>
-  </si>
-  <si>
     <t>[0,value,channel_value]</t>
   </si>
   <si>
@@ -641,6 +635,54 @@
   </si>
   <si>
     <t>[0,bool,toggle_input, rising_edge]</t>
+  </si>
+  <si>
+    <t>A standard XOR-Gate. If the inputs a different, returns true</t>
+  </si>
+  <si>
+    <t>Control your Philips Hue Lux Lamps (white ones only)</t>
+  </si>
+  <si>
+    <t>Performs basic math operations (+ , -, *, /, min, max, mod, pow)</t>
+  </si>
+  <si>
+    <t>With this node you can get Weatherdata from the OpenWeatherMap Service, to use this node you must create a account on the Servicewebsite</t>
+  </si>
+  <si>
+    <t>This node serarch until the needlestring and returns the both splitted parts.</t>
+  </si>
+  <si>
+    <t>With this node you can remove a spcific lenght of the start of the string.</t>
+  </si>
+  <si>
+    <t>This node increments the output value with a specific value at a rising edge</t>
+  </si>
+  <si>
+    <t>This gate returns his input</t>
+  </si>
+  <si>
+    <t>This gate inverts his input</t>
+  </si>
+  <si>
+    <t>This gate represents a Reset/Set logic gatter.Set the output to true with a rising edge on the set input , or to false with a rising edge on the reset input</t>
+  </si>
+  <si>
+    <t>This gate represents a T-FlipFlop logic gate. With a rising edge on the input you can toggle the output value</t>
+  </si>
+  <si>
+    <t>This node converts a int value to an string value</t>
+  </si>
+  <si>
+    <t>This node converts a string value to an float value</t>
+  </si>
+  <si>
+    <t>This node converts a string value to an int value</t>
+  </si>
+  <si>
+    <t>This node converts a float value to an string value</t>
+  </si>
+  <si>
+    <t>This node converts a float value to an int value</t>
   </si>
 </sst>
 </file>
@@ -679,7 +721,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -690,12 +732,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFEEEEEE"/>
-        <bgColor rgb="FFEEEEEE"/>
       </patternFill>
     </fill>
     <fill>
@@ -714,6 +750,18 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFEEEEEE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -744,7 +792,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -764,25 +812,28 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1088,8 +1139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1113,13 +1164,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -1128,7 +1179,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
@@ -1171,13 +1222,13 @@
         <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E2" s="3" t="b">
         <v>1</v>
@@ -1194,7 +1245,7 @@
       <c r="I2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="11"/>
+      <c r="J2" s="9"/>
       <c r="K2" s="3" t="s">
         <v>13</v>
       </c>
@@ -1210,13 +1261,13 @@
         <v>16</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E3" s="3" t="b">
         <v>1</v>
@@ -1236,7 +1287,7 @@
       <c r="J3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="10"/>
+      <c r="K3" s="8"/>
       <c r="L3" s="3" t="s">
         <v>14</v>
       </c>
@@ -1249,13 +1300,13 @@
         <v>21</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E4" s="3" t="b">
         <v>1</v>
@@ -1273,14 +1324,14 @@
         <v>23</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="K4" s="11"/>
+        <v>147</v>
+      </c>
+      <c r="K4" s="9"/>
       <c r="L4" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="M4" s="4" t="s">
         <v>152</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1288,13 +1339,13 @@
         <v>24</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E5" s="3" t="b">
         <v>1</v>
@@ -1312,14 +1363,14 @@
         <v>23</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="K5" s="11"/>
+        <v>148</v>
+      </c>
+      <c r="K5" s="9"/>
       <c r="L5" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="M5" s="4" t="s">
         <v>151</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1327,13 +1378,13 @@
         <v>26</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E6" s="3" t="b">
         <v>0</v>
@@ -1356,9 +1407,9 @@
       <c r="K6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="L6" s="11"/>
+      <c r="L6" s="9"/>
       <c r="M6" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1366,13 +1417,13 @@
         <v>31</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E7" s="3" t="b">
         <v>0</v>
@@ -1395,9 +1446,9 @@
       <c r="K7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="L7" s="11"/>
+      <c r="L7" s="9"/>
       <c r="M7" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1405,13 +1456,13 @@
         <v>33</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E8" s="3" t="b">
         <v>0</v>
@@ -1434,22 +1485,24 @@
       <c r="K8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="L8" s="12"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="7"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="N8" s="13"/>
     </row>
     <row r="9" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>36</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E9" s="3" t="b">
         <v>0</v>
@@ -1460,7 +1513,7 @@
       <c r="G9" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H9" s="8" t="b">
+      <c r="H9" s="6" t="b">
         <v>1</v>
       </c>
       <c r="I9" s="3" t="s">
@@ -1469,23 +1522,26 @@
       <c r="J9" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="K9" s="9" t="s">
+      <c r="K9" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="11"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="2" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="10" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E10" s="3" t="b">
         <v>0</v>
@@ -1508,20 +1564,23 @@
       <c r="K10" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="L10" s="11"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="2" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="11" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E11" s="3" t="b">
         <v>0</v>
@@ -1544,20 +1603,20 @@
       <c r="K11" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="L11" s="13"/>
+      <c r="L11" s="11"/>
     </row>
     <row r="12" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>46</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E12" s="3" t="b">
         <v>0</v>
@@ -1580,20 +1639,20 @@
       <c r="K12" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="L12" s="11"/>
+      <c r="L12" s="9"/>
     </row>
     <row r="13" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>50</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E13" s="3" t="b">
         <v>0</v>
@@ -1616,20 +1675,20 @@
       <c r="K13" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="L13" s="11"/>
+      <c r="L13" s="9"/>
     </row>
     <row r="14" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>54</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E14" s="3" t="b">
         <v>0</v>
@@ -1647,13 +1706,13 @@
         <v>28</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="K14" s="4" t="s">
         <v>30</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="15" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1661,13 +1720,13 @@
         <v>55</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>56</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E15" s="3" t="b">
         <v>0</v>
@@ -1685,13 +1744,13 @@
         <v>28</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="K15" s="4" t="s">
         <v>30</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="16" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1699,13 +1758,13 @@
         <v>57</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>58</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E16" s="3" t="b">
         <v>0</v>
@@ -1723,13 +1782,13 @@
         <v>28</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="K16" s="4" t="s">
         <v>30</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1737,13 +1796,13 @@
         <v>59</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>60</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E17" s="3" t="b">
         <v>0</v>
@@ -1761,25 +1820,28 @@
         <v>28</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="K17" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="L17" s="11"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="2" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="18" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>61</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>62</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E18" s="3" t="b">
         <v>0</v>
@@ -1797,25 +1859,28 @@
         <v>28</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="K18" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="L18" s="11"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="2" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="19" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>63</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E19" s="3" t="b">
         <v>0</v>
@@ -1832,12 +1897,12 @@
       <c r="I19" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J19" s="11"/>
+      <c r="J19" s="9"/>
       <c r="K19" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1845,13 +1910,13 @@
         <v>65</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>66</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E20" s="3" t="b">
         <v>0</v>
@@ -1868,12 +1933,12 @@
       <c r="I20" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J20" s="11"/>
+      <c r="J20" s="9"/>
       <c r="K20" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1881,13 +1946,13 @@
         <v>67</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>68</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E21" s="3" t="b">
         <v>0</v>
@@ -1904,12 +1969,12 @@
       <c r="I21" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J21" s="11"/>
+      <c r="J21" s="9"/>
       <c r="K21" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1917,13 +1982,13 @@
         <v>69</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>70</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E22" s="3" t="b">
         <v>0</v>
@@ -1940,24 +2005,24 @@
       <c r="I22" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J22" s="11"/>
+      <c r="J22" s="9"/>
       <c r="K22" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="L22" s="11"/>
+        <v>174</v>
+      </c>
+      <c r="L22" s="9"/>
     </row>
     <row r="23" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>71</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>72</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E23" s="3" t="b">
         <v>0</v>
@@ -1974,24 +2039,24 @@
       <c r="I23" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J23" s="11"/>
+      <c r="J23" s="9"/>
       <c r="K23" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="L23" s="11"/>
+        <v>175</v>
+      </c>
+      <c r="L23" s="9"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>73</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>74</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E24" s="3" t="b">
         <v>0</v>
@@ -2009,25 +2074,28 @@
         <v>28</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="L24" s="11"/>
+        <v>169</v>
+      </c>
+      <c r="L24" s="9"/>
+      <c r="M24" s="2" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="25" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>75</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>76</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E25" s="3" t="b">
         <v>0</v>
@@ -2045,25 +2113,28 @@
         <v>28</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="L25" s="11"/>
+        <v>170</v>
+      </c>
+      <c r="L25" s="9"/>
+      <c r="M25" s="2" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="26" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>77</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>78</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E26" s="3" t="b">
         <v>0</v>
@@ -2081,25 +2152,28 @@
         <v>28</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="L26" s="11"/>
+        <v>169</v>
+      </c>
+      <c r="L26" s="9"/>
+      <c r="M26" s="2" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="27" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>79</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>80</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E27" s="3" t="b">
         <v>0</v>
@@ -2117,25 +2191,28 @@
         <v>28</v>
       </c>
       <c r="J27" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="K27" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="K27" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="L27" s="11"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="2" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="28" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>81</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>78</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E28" s="3" t="b">
         <v>0</v>
@@ -2153,25 +2230,28 @@
         <v>28</v>
       </c>
       <c r="J28" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="K28" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="K28" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="L28" s="11"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="2" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="29" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>82</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>83</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E29" s="3" t="b">
         <v>0</v>
@@ -2189,25 +2269,28 @@
         <v>28</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="L29" s="11"/>
+        <v>168</v>
+      </c>
+      <c r="L29" s="9"/>
+      <c r="M29" s="2" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="30" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>84</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>85</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E30" s="3" t="b">
         <v>0</v>
@@ -2224,11 +2307,11 @@
       <c r="I30" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J30" s="11"/>
+      <c r="J30" s="9"/>
       <c r="K30" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="L30" s="11"/>
+      <c r="L30" s="9"/>
       <c r="M30" s="3" t="s">
         <v>87</v>
       </c>
@@ -2238,13 +2321,13 @@
         <v>88</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>89</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E31" s="3" t="b">
         <v>0</v>
@@ -2262,10 +2345,10 @@
         <v>28</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="M31" s="3" t="s">
         <v>90</v>
@@ -2276,13 +2359,13 @@
         <v>91</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>92</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E32" s="3" t="b">
         <v>0</v>
@@ -2305,7 +2388,7 @@
       <c r="K32" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="L32" s="11"/>
+      <c r="L32" s="9"/>
       <c r="M32" s="3" t="s">
         <v>95</v>
       </c>
@@ -2315,13 +2398,13 @@
         <v>96</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>97</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E33" s="3" t="b">
         <v>0</v>
@@ -2338,29 +2421,29 @@
       <c r="I33" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="J33" s="9" t="s">
+      <c r="J33" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="K33" s="11"/>
+      <c r="K33" s="9"/>
       <c r="L33" s="3" t="s">
         <v>100</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>101</v>
+        <v>208</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>103</v>
-      </c>
       <c r="D34" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E34" s="3" t="b">
         <v>0</v>
@@ -2378,203 +2461,215 @@
         <v>28</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="D35" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="E35" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F35" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G35" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H35" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="K35" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="L35" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="M35" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="E35" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F35" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G35" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H35" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I35" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J35" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="K35" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="L35" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="M35" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
+      <c r="B36" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="C36" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="D36" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="E36" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F36" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G36" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H36" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J36" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="E36" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F36" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G36" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H36" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I36" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J36" s="4" t="s">
+      <c r="K36" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="K36" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="L36" s="11"/>
+      <c r="L36" s="9"/>
+      <c r="M36" s="2" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="37" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E37" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F37" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G37" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H37" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J37" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="C37" s="3" t="s">
+      <c r="K37" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="D37" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="E37" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F37" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G37" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H37" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I37" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J37" s="4" t="s">
+      <c r="L37" s="9"/>
+      <c r="M37" s="4" t="s">
         <v>158</v>
-      </c>
-      <c r="K37" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="L37" s="11"/>
-      <c r="M37" s="4" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B38" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E38" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F38" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G38" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H38" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J38" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="K38" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="D38" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="E38" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F38" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G38" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H38" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I38" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J38" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="K38" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="L38" s="11"/>
+      <c r="L38" s="9"/>
+      <c r="M38" s="2" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="39" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E39" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F39" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G39" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H39" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="K39" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="B39" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="E39" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F39" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G39" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H39" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I39" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J39" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="K39" s="4" t="s">
-        <v>185</v>
-      </c>
       <c r="L39" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
+      </c>
+      <c r="M39" s="2" t="s">
+        <v>211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>